<commit_message>
File changed so that now we have mechanism to prevent combination for Assignee and No Access participant for a Complaint
</commit_message>
<xml_diff>
--- a/acm/rules/drools-participant-assignment-rules.xlsx
+++ b/acm/rules/drools-participant-assignment-rules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>RuleSet</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>participants != null &amp;&amp; participants.containsKey('No Access') &amp;&amp; participants.containsKey('assignee')</t>
+  </si>
+  <si>
+    <t>Complaint - Check participants list for NoAccess &amp; Owner</t>
   </si>
 </sst>
 </file>
@@ -786,10 +789,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,6 +1021,23 @@
         <v>41</v>
       </c>
       <c r="F20" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated rules for participants. Now if there is a more than one owner, or more then one owning group the rules will fire and with that, we will prevent the creation of that entity.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-participant-assignment-rules.xlsx
+++ b/acm/rules/drools-participant-assignment-rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojan.milenkoski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovan.ivanovski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>RuleSet</t>
   </si>
@@ -198,6 +198,75 @@
   </si>
   <si>
     <t>PERSON</t>
+  </si>
+  <si>
+    <t>Case File -Check if entry exists for participant Type assignee already exists</t>
+  </si>
+  <si>
+    <t>Only one Assignee allowed</t>
+  </si>
+  <si>
+    <t>Case file -Check if entry exists for participant Type owner already exists</t>
+  </si>
+  <si>
+    <t>Only one owner allowed</t>
+  </si>
+  <si>
+    <t>Case file -Check if entry exists for participant Type owningGroup already exists</t>
+  </si>
+  <si>
+    <t>Only one owning group allowed</t>
+  </si>
+  <si>
+    <t>Complaints -Check if entry exists for participant Type assignee already exists</t>
+  </si>
+  <si>
+    <t>Complaints -Check if entry exists for participant Type owner already exists</t>
+  </si>
+  <si>
+    <t>Complaints -Check if entry exists for participant Type owningGroup already exists</t>
+  </si>
+  <si>
+    <t>People -Check if entry exists for participant Type assignee already exists</t>
+  </si>
+  <si>
+    <t>People -Check if entry exists for participant Type owner already exists</t>
+  </si>
+  <si>
+    <t>People -Check if entry exists for participant Type owningGroup already exists</t>
+  </si>
+  <si>
+    <t>Organization -Check if entry exists for participant Type assignee already exists</t>
+  </si>
+  <si>
+    <t>Organization -Check if entry exists for participant Type owner already exists</t>
+  </si>
+  <si>
+    <t>Organization -Check if entry exists for participant Type owningGroup already exists</t>
+  </si>
+  <si>
+    <t>Documents -Check if entry exists for participant Type assignee already exists</t>
+  </si>
+  <si>
+    <t>DOC_REPO</t>
+  </si>
+  <si>
+    <t>Documents -Check if entry exists for participant Type owner already exists</t>
+  </si>
+  <si>
+    <t>Documents -Check if entry exists for participant Type owningGroup already exists</t>
+  </si>
+  <si>
+    <t>participants != null &amp;&amp; participants.containsKey('assignee') &amp;&amp; participants['assignee'].size() &gt;1</t>
+  </si>
+  <si>
+    <t>participants != null &amp;&amp; participants.containsKey('owner') &amp;&amp; participants['owner'].size() &gt;1</t>
+  </si>
+  <si>
+    <t>participants != null &amp;&amp; participants.containsKey('owning group') &amp;&amp; participants['owning group'].size() &gt;1</t>
+  </si>
+  <si>
+    <t>participants != null &amp;&amp; participants.containsKey('assignee') &amp;&amp; participants['assignee'].size()&gt;1</t>
   </si>
 </sst>
 </file>
@@ -397,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -423,6 +492,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -810,10 +883,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,6 +1167,231 @@
       </c>
       <c r="F23" s="13" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B37" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B38" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>